<commit_message>
Commodities and Shipper Contact Script updated
</commit_message>
<xml_diff>
--- a/TestData/Commodities.xlsx
+++ b/TestData/Commodities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="AddCommodities" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="50">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -128,6 +128,45 @@
   </si>
   <si>
     <t>Edit</t>
+  </si>
+  <si>
+    <t>Invalid_AddCommodity_TC001</t>
+  </si>
+  <si>
+    <t>Unable to add commodity</t>
+  </si>
+  <si>
+    <t>the upper limit is required</t>
+  </si>
+  <si>
+    <t>the lower limit is required</t>
+  </si>
+  <si>
+    <t>7000</t>
+  </si>
+  <si>
+    <t>the commodity name is required</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>Invalid_AddCommodity_TC001(2)</t>
+  </si>
+  <si>
+    <t>Invalid_AddCommodity_TC001(3)</t>
+  </si>
+  <si>
+    <t>Invalid_AddCommodity_TC001(4)</t>
+  </si>
+  <si>
+    <t>Invalid_AddCommodity_TC001(5)</t>
+  </si>
+  <si>
+    <t>Invalid_AddCommodity_TC001(6)</t>
+  </si>
+  <si>
+    <t>the upper limit must be greater than the lower limit</t>
   </si>
 </sst>
 </file>
@@ -491,16 +530,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,6 +618,144 @@
       </c>
       <c r="G3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -592,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -670,10 +849,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +912,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -743,7 +936,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>